<commit_message>
feat: qa-level-1-planning-analysis >> add product map section
</commit_message>
<xml_diff>
--- a/documents/qa-example.xlsx
+++ b/documents/qa-example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myProjects\page404\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myProjects\dictionary\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -424,32 +424,6 @@
     <t>Тестирование адаптивности</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Чек-лист</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-КАРТА САЙТА</t>
-    </r>
-  </si>
-  <si>
     <t>Шаги</t>
   </si>
   <si>
@@ -605,6 +579,9 @@
   </si>
   <si>
     <t>продолжительность, кал.дней</t>
+  </si>
+  <si>
+    <t>Чек-лист</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1019,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1181,6 +1158,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1238,38 +1233,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1560,7 +1540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1615,12 +1597,12 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1664,13 +1646,13 @@
         <v>97</v>
       </c>
       <c r="C1" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="42" t="s">
         <v>106</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1678,16 +1660,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="49" t="s">
-        <v>134</v>
-      </c>
       <c r="D2" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="49" t="s">
         <v>131</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1728,92 +1710,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="80" t="s">
         <v>148</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="82" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="82"/>
+      <c r="F5" s="43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="55" t="s">
         <v>135</v>
-      </c>
-      <c r="B5" s="78" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="79" t="s">
-        <v>146</v>
-      </c>
-      <c r="E5" s="79"/>
-      <c r="F5" s="43" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="74" t="s">
-        <v>136</v>
       </c>
       <c r="B6" s="43">
         <v>20</v>
       </c>
-      <c r="D6" s="77" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="77"/>
-      <c r="F6" s="83">
+      <c r="D6" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="83"/>
+      <c r="F6" s="59">
         <v>43871</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
-        <v>137</v>
+      <c r="A7" s="55" t="s">
+        <v>136</v>
       </c>
       <c r="B7" s="43">
         <v>8</v>
       </c>
-      <c r="D7" s="77" t="s">
-        <v>145</v>
-      </c>
-      <c r="E7" s="77"/>
-      <c r="F7" s="83">
+      <c r="D7" s="83" t="s">
+        <v>144</v>
+      </c>
+      <c r="E7" s="83"/>
+      <c r="F7" s="59">
         <v>43876</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="74" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="82">
+      <c r="A8" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="B8" s="58">
         <f>100-(B7/B6*100)</f>
         <v>60</v>
       </c>
-      <c r="D8" s="77" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="77"/>
+      <c r="D8" s="83" t="s">
+        <v>151</v>
+      </c>
+      <c r="E8" s="83"/>
       <c r="F8" s="43">
         <f>F7-F6</f>
         <v>5</v>
@@ -1821,31 +1803,31 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="78" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="78"/>
+      <c r="D10" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="72" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="43" t="s">
-        <v>141</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="F10" s="43" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="72">
+      <c r="B11" s="78">
         <f>SUM(D11:F11)</f>
         <v>15</v>
       </c>
-      <c r="C11" s="72"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="43">
         <v>2</v>
       </c>
@@ -1857,14 +1839,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="74" t="s">
-        <v>140</v>
-      </c>
-      <c r="B12" s="72">
+      <c r="A12" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" s="78">
         <f>SUM(D12:F12)</f>
         <v>8</v>
       </c>
-      <c r="C12" s="72"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="43">
         <v>1</v>
       </c>
@@ -1876,23 +1858,23 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
-        <v>147</v>
-      </c>
-      <c r="B13" s="80">
+      <c r="A13" s="55" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="81">
         <f>100-(B12/B11*100)</f>
         <v>46.666666666666664</v>
       </c>
-      <c r="C13" s="80"/>
-      <c r="D13" s="81">
+      <c r="C13" s="81"/>
+      <c r="D13" s="57">
         <f t="shared" ref="D13:E13" si="0">100-(D12/D11*100)</f>
         <v>50</v>
       </c>
-      <c r="E13" s="81">
+      <c r="E13" s="57">
         <f t="shared" si="0"/>
         <v>33.333333333333343</v>
       </c>
-      <c r="F13" s="81">
+      <c r="F13" s="57">
         <f>100-(F12/F11*100)</f>
         <v>50</v>
       </c>
@@ -1904,17 +1886,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B15" location="СОДЕРЖАНИЕ!A1" display="СОДЕРЖАНИЕ"/>
@@ -2230,11 +2212,11 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
       <c r="E5" s="4">
         <f>SUM(E2:E4)</f>
         <v>34</v>
@@ -2244,11 +2226,11 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="56"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="62"/>
       <c r="E6" s="4">
         <v>5</v>
       </c>
@@ -2257,11 +2239,11 @@
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="56"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="5">
         <f>E5*E6</f>
         <v>170</v>
@@ -2370,10 +2352,10 @@
       <c r="A18" s="16">
         <v>7</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="57"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="12">
         <f>SUM(D12:D17)</f>
         <v>310</v>
@@ -2414,32 +2396,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="59"/>
-      <c r="F1" s="58" t="s">
+      <c r="E1" s="65"/>
+      <c r="F1" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="H1" s="58" t="s">
+      <c r="G1" s="65"/>
+      <c r="H1" s="64" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="59"/>
+      <c r="I1" s="65"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
       <c r="D2" s="17" t="s">
         <v>48</v>
       </c>
@@ -2460,7 +2442,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="73">
+      <c r="A3" s="54">
         <v>1</v>
       </c>
       <c r="B3" s="18" t="s">
@@ -2489,7 +2471,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="73">
+      <c r="A4" s="54">
         <v>2</v>
       </c>
       <c r="B4" s="18"/>
@@ -2502,7 +2484,7 @@
       <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="73">
+      <c r="A5" s="54">
         <v>3</v>
       </c>
       <c r="B5" s="18"/>
@@ -2554,10 +2536,10 @@
       <c r="A1" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="68"/>
+      <c r="C1" s="74"/>
       <c r="D1" s="36" t="s">
         <v>67</v>
       </c>
@@ -2590,10 +2572,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="68" t="s">
         <v>83</v>
       </c>
       <c r="C2" s="23" t="s">
@@ -2613,8 +2595,8 @@
       <c r="M2" s="33"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="63"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="69"/>
       <c r="C3" s="24" t="s">
         <v>78</v>
       </c>
@@ -2632,8 +2614,8 @@
       <c r="M3" s="34"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="65"/>
-      <c r="B4" s="63" t="s">
+      <c r="A4" s="71"/>
+      <c r="B4" s="69" t="s">
         <v>84</v>
       </c>
       <c r="C4" s="25" t="s">
@@ -2653,8 +2635,8 @@
       <c r="M4" s="34"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="65"/>
-      <c r="B5" s="63"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="69"/>
       <c r="C5" s="24" t="s">
         <v>78</v>
       </c>
@@ -2672,7 +2654,7 @@
       <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="39" t="s">
         <v>94</v>
       </c>
@@ -2703,10 +2685,10 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="68" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -2726,8 +2708,8 @@
       <c r="M7" s="33"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="65"/>
-      <c r="B8" s="63"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="24" t="s">
         <v>78</v>
       </c>
@@ -2745,8 +2727,8 @@
       <c r="M8" s="34"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
-      <c r="B9" s="63" t="s">
+      <c r="A9" s="71"/>
+      <c r="B9" s="69" t="s">
         <v>86</v>
       </c>
       <c r="C9" s="25" t="s">
@@ -2766,8 +2748,8 @@
       <c r="M9" s="34"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="71"/>
+      <c r="B10" s="69"/>
       <c r="C10" s="24" t="s">
         <v>78</v>
       </c>
@@ -2785,7 +2767,7 @@
       <c r="M10" s="34"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="66"/>
+      <c r="A11" s="72"/>
       <c r="B11" s="39" t="s">
         <v>94</v>
       </c>
@@ -2816,10 +2798,10 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="68" t="s">
         <v>87</v>
       </c>
       <c r="C12" s="23" t="s">
@@ -2839,8 +2821,8 @@
       <c r="M12" s="33"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="65"/>
-      <c r="B13" s="63"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="69"/>
       <c r="C13" s="24" t="s">
         <v>78</v>
       </c>
@@ -2858,7 +2840,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="66"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="39" t="s">
         <v>94</v>
       </c>
@@ -2963,28 +2945,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="71"/>
+      <c r="A1" s="84" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="77"/>
       <c r="C1" s="47"/>
       <c r="D1" s="47"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="69"/>
+      <c r="D2" s="75"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
+      <c r="A3" s="76"/>
+      <c r="B3" s="76"/>
       <c r="C3" s="44">
         <v>43871</v>
       </c>
@@ -3096,10 +3078,10 @@
         <v>97</v>
       </c>
       <c r="C1" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="40" t="s">
         <v>106</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -3107,13 +3089,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="120" x14ac:dyDescent="0.25">
@@ -3121,13 +3103,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3158,29 +3140,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="72"/>
+      <c r="A1" s="78" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="78"/>
       <c r="C1" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="E1" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="F1" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="G1" s="50" t="s">
         <v>115</v>
-      </c>
-      <c r="G1" s="50" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" s="52">
         <f>SUM(C2:G2)</f>
@@ -3209,7 +3191,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" s="16">
         <f>SUM(C3:G3)</f>
@@ -3225,7 +3207,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="16">
         <f t="shared" ref="B4:B9" si="1">SUM(C4:G4)</f>
@@ -3241,7 +3223,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="16">
         <f t="shared" si="1"/>
@@ -3259,7 +3241,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="16">
         <f t="shared" si="1"/>
@@ -3275,7 +3257,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="16">
         <f t="shared" si="1"/>
@@ -3291,7 +3273,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="16">
         <f t="shared" si="1"/>
@@ -3307,7 +3289,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="16">
         <f t="shared" si="1"/>
@@ -3323,26 +3305,26 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" s="52">
         <f>SUM(B3:B9)</f>
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>